<commit_message>
Criando tabela para o chat
</commit_message>
<xml_diff>
--- a/Auxiliar/DicionárioGetDevWEB.xlsx
+++ b/Auxiliar/DicionárioGetDevWEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\N8\GetDev-WEB\Auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB345C87-071D-4F01-A8B7-884A3E89B8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FF785B-59BC-43EC-ACE9-2C5D5B6FC344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2FE1E48A-CC93-4FF6-9009-E3FC4E2BD670}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="94">
   <si>
     <t>Linguagem</t>
   </si>
@@ -291,6 +291,33 @@
   </si>
   <si>
     <t>Servico</t>
+  </si>
+  <si>
+    <t>Mensagem</t>
+  </si>
+  <si>
+    <t>id_Mensagem</t>
+  </si>
+  <si>
+    <t>id_Proposta_Mensagem</t>
+  </si>
+  <si>
+    <t>texto_Mensagem</t>
+  </si>
+  <si>
+    <t>registro_Mensagem</t>
+  </si>
+  <si>
+    <t>remetente_Mensagem</t>
+  </si>
+  <si>
+    <t>status_Mensagem</t>
+  </si>
+  <si>
+    <t>obs_Mensagem</t>
+  </si>
+  <si>
+    <t>arquivo_Mensagem</t>
   </si>
 </sst>
 </file>
@@ -306,18 +333,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -334,7 +355,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FDD7268-EFCE-4D26-BD69-25E2771A0B3A}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,6 +1672,149 @@
         <v>14</v>
       </c>
     </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89" t="s">
+        <v>28</v>
+      </c>
+      <c r="D89" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>